<commit_message>
Renamed passives in order of increasing value, highlighted parts needed in bom
</commit_message>
<xml_diff>
--- a/hardware/observer/rev_b/observer_bom.xlsx
+++ b/hardware/observer/rev_b/observer_bom.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neals_000\Documents\git\observer\hardware\observer\rev_b\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nealjack\Documents\git\observer\hardware\observer\rev_b\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11655"/>
   </bookViews>
   <sheets>
     <sheet name="observer_bom" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="115">
   <si>
     <t>Qty</t>
   </si>
@@ -51,9 +51,6 @@
     <t>0402_CAP</t>
   </si>
   <si>
-    <t>C13</t>
-  </si>
-  <si>
     <t>0402 Capacitor</t>
   </si>
   <si>
@@ -90,18 +87,12 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>C20</t>
-  </si>
-  <si>
     <t>445-8919-1-ND</t>
   </si>
   <si>
     <t>1M</t>
   </si>
   <si>
-    <t>R9</t>
-  </si>
-  <si>
     <t>2.2k</t>
   </si>
   <si>
@@ -120,9 +111,6 @@
     <t>CAP0603</t>
   </si>
   <si>
-    <t>C10</t>
-  </si>
-  <si>
     <t>511-1493-1-ND</t>
   </si>
   <si>
@@ -135,21 +123,12 @@
     <t>4.7uF</t>
   </si>
   <si>
-    <t>C11, C12, C15</t>
-  </si>
-  <si>
     <t>470pF</t>
   </si>
   <si>
-    <t>C14</t>
-  </si>
-  <si>
     <t>5k</t>
   </si>
   <si>
-    <t>R11</t>
-  </si>
-  <si>
     <t>ADC121C021</t>
   </si>
   <si>
@@ -348,24 +327,6 @@
     <t>Electret microphone</t>
   </si>
   <si>
-    <t>PINHD-1X1</t>
-  </si>
-  <si>
-    <t>1X01</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>PIN HEADER</t>
-  </si>
-  <si>
-    <t>C2, C3, C4, C5, C6, C7, C8, C16, C17</t>
-  </si>
-  <si>
-    <t>R2, R4, R5, R6, R7, R8</t>
-  </si>
-  <si>
     <t>0603 Capacitor</t>
   </si>
   <si>
@@ -376,6 +337,33 @@
   </si>
   <si>
     <t>2x08 pin header</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4, C5, C6, C7, C8, C9, C10, C11, C12</t>
+  </si>
+  <si>
+    <t>C13, C14, C15</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5, R6, R7, R8, R9</t>
   </si>
 </sst>
 </file>
@@ -518,7 +506,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -696,6 +684,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -859,8 +853,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1182,22 +1177,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.36328125" customWidth="1"/>
-    <col min="3" max="3" width="34.90625" customWidth="1"/>
-    <col min="4" max="4" width="26.90625" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
-    <col min="6" max="6" width="43.36328125" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1220,52 +1215,52 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1274,21 +1269,21 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -1297,41 +1292,41 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -1340,59 +1335,59 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>115</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1400,477 +1395,460 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
       </c>
       <c r="E13" t="s">
         <v>114</v>
       </c>
       <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
         <v>20</v>
       </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
         <v>68</v>
       </c>
-      <c r="F15" t="s">
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
         <v>69</v>
       </c>
-      <c r="G15" t="s">
+      <c r="E16" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="F22" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E16" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" t="s">
-        <v>97</v>
-      </c>
-      <c r="E18" t="s">
+    </row>
+    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F18" t="s">
+      <c r="D24" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G18" t="s">
+      <c r="E24" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" t="s">
-        <v>106</v>
-      </c>
-      <c r="E24" t="s">
-        <v>107</v>
-      </c>
-      <c r="F24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F24" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D28" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="F30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F31" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>109</v>
-      </c>
-      <c r="D32" t="s">
-        <v>110</v>
-      </c>
-      <c r="E32" t="s">
-        <v>111</v>
-      </c>
-      <c r="F32" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added all missing digikey part numbers new parts highlighted in orange
</commit_message>
<xml_diff>
--- a/hardware/observer/rev_b/observer_bom.xlsx
+++ b/hardware/observer/rev_b/observer_bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="125">
   <si>
     <t>Qty</t>
   </si>
@@ -126,9 +126,6 @@
     <t>470pF</t>
   </si>
   <si>
-    <t>5k</t>
-  </si>
-  <si>
     <t>ADC121C021</t>
   </si>
   <si>
@@ -324,9 +321,6 @@
     <t>Q1</t>
   </si>
   <si>
-    <t>Electret microphone</t>
-  </si>
-  <si>
     <t>0603 Capacitor</t>
   </si>
   <si>
@@ -364,13 +358,49 @@
   </si>
   <si>
     <t>R5, R6, R7, R8, R9</t>
+  </si>
+  <si>
+    <t>490-6197-1-ND</t>
+  </si>
+  <si>
+    <t>490-8208-1-ND</t>
+  </si>
+  <si>
+    <t>490-5915-1-ND</t>
+  </si>
+  <si>
+    <t>RHM22.0CDCT-ND</t>
+  </si>
+  <si>
+    <t>RHM2.2KCECT-ND</t>
+  </si>
+  <si>
+    <t>4.99k</t>
+  </si>
+  <si>
+    <t>P4.99KLCT-ND</t>
+  </si>
+  <si>
+    <t>RHM1.0MCECT-ND</t>
+  </si>
+  <si>
+    <t>OPA344NACT-ND</t>
+  </si>
+  <si>
+    <t>ADC121C021CIMK/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>102-1721-ND</t>
+  </si>
+  <si>
+    <t>CMA-4544PF-W Electret microphone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,6 +535,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -688,7 +724,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -853,9 +889,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1179,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1226,7 @@
     <col min="3" max="3" width="34.85546875" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="6" max="6" width="43.42578125" customWidth="1"/>
+    <col min="6" max="6" width="66.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1234,6 +1271,9 @@
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1249,11 +1289,14 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1269,7 +1312,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -1292,7 +1335,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -1315,11 +1358,14 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1335,7 +1381,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -1358,10 +1404,10 @@
         <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
         <v>30</v>
@@ -1386,6 +1432,9 @@
       <c r="F9" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G9" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1401,7 +1450,7 @@
         <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -1429,13 +1478,16 @@
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
@@ -1444,10 +1496,13 @@
         <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1464,7 +1519,7 @@
         <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F13" t="s">
         <v>19</v>
@@ -1492,28 +1547,31 @@
       <c r="F14" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G14" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
         <v>59</v>
       </c>
-      <c r="C15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>60</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>61</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>62</v>
-      </c>
-      <c r="G15" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1521,22 +1579,22 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
         <v>68</v>
       </c>
-      <c r="C16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>69</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>70</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>71</v>
-      </c>
-      <c r="G16" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1544,22 +1602,22 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
         <v>84</v>
       </c>
-      <c r="C17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>85</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>86</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>87</v>
-      </c>
-      <c r="G17" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1567,22 +1625,22 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" t="s">
         <v>89</v>
       </c>
-      <c r="C18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>90</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>91</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>92</v>
-      </c>
-      <c r="G18" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1590,19 +1648,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s">
         <v>43</v>
       </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>44</v>
-      </c>
-      <c r="F19" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1610,22 +1668,22 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
         <v>38</v>
       </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>39</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>40</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>41</v>
-      </c>
-      <c r="G20" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1633,19 +1691,19 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>49</v>
-      </c>
-      <c r="F21" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1653,19 +1711,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>76</v>
+      <c r="G22" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1673,19 +1734,22 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1693,16 +1757,19 @@
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>101</v>
+        <v>124</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1710,22 +1777,22 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
         <v>55</v>
       </c>
-      <c r="C25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>56</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" t="s">
         <v>57</v>
-      </c>
-      <c r="F25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1733,19 +1800,19 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
         <v>51</v>
       </c>
-      <c r="C26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>52</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>53</v>
-      </c>
-      <c r="F26" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1753,19 +1820,19 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" t="s">
         <v>77</v>
       </c>
-      <c r="C27" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>78</v>
       </c>
-      <c r="E27" t="s">
-        <v>79</v>
-      </c>
       <c r="F27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1773,19 +1840,19 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" t="s">
         <v>94</v>
       </c>
-      <c r="C28" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>95</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>96</v>
-      </c>
-      <c r="F28" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1793,19 +1860,19 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" t="s">
         <v>64</v>
       </c>
-      <c r="C29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>65</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>66</v>
-      </c>
-      <c r="F29" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1813,19 +1880,19 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" t="s">
         <v>46</v>
-      </c>
-      <c r="C30" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" t="s">
-        <v>103</v>
-      </c>
-      <c r="F30" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1833,25 +1900,26 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" t="s">
         <v>80</v>
       </c>
-      <c r="C31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>81</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>82</v>
-      </c>
-      <c r="G31" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>